<commit_message>
All 4 test cases Code
</commit_message>
<xml_diff>
--- a/reports/Extent-Report/Zlaata-QAResults.xlsx
+++ b/reports/Extent-Report/Zlaata-QAResults.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="79">
   <si>
     <t>Duration</t>
   </si>
@@ -229,112 +229,47 @@
     <t>DEVICE NAME</t>
   </si>
   <si>
-    <t>Sept 20, 2025 5:46:11 pm</t>
+    <t>Sept 23, 2025 9:56:37 am</t>
   </si>
   <si>
-    <t>Sept 20, 2025 5:41:00 pm</t>
+    <t>Sept 23, 2025 9:54:58 am</t>
   </si>
   <si>
-    <t>Sept 20, 2025 5:46:07 pm</t>
+    <t>Sept 23, 2025 9:56:33 am</t>
   </si>
   <si>
-    <t>5 m 7.108 s</t>
+    <t>1 m 35.193 s</t>
   </si>
   <si>
     <t>0%</t>
   </si>
   <si>
-    <t>67%</t>
+    <t>75%</t>
   </si>
   <si>
-    <t>@TC_UI_Zlaata_ASP_04</t>
+    <t>@TC_UI_Zlaata_EEF_04</t>
   </si>
   <si>
-    <t>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</t>
+    <t>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</t>
   </si>
   <si>
-    <t>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</t>
+    <t>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</t>
   </si>
   <si>
-    <t>5 m 6.272 s</t>
+    <t>1 m 34.452 s</t>
   </si>
   <si>
-    <t>5 m 6.277 s</t>
+    <t>1 m 34.460 s</t>
   </si>
   <si>
-    <t>Then I should see the same product appear first in the User Application Micro Page</t>
+    <t>Then I verify both exported inactive products files "InactiveProducts1.xlsx" and "InactiveProducts2.xlsx" have matching product names</t>
   </si>
   <si>
-    <t xml:space="preserve">org.openqa.selenium.NoSuchWindowException: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=140.0.7339.129)
-Build info: version: '4.34.0', revision: '707dcb4246*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.8'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [6f42af8d51a245b62f759c30c0cc94cf, findElements {value=//div[@id='cls_newproduct_sec_dev']/div[contains(@class,'product_list_cards_list')][1]//h2[@class='product_list_cards_heading'], using=xpath}]
-Capabilities {acceptInsecureCerts: true, browserName: chrome, browserVersion: 140.0.7339.129, chrome: {chromedriverVersion: 140.0.7339.185 (eeea00e459e..., userDataDir: C:\Users\SAROJK~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52687}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52687/devtoo..., se:cdpVersion: 140.0.7339.129, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 6f42af8d51a245b62f759c30c0cc94cf
-	at java.base/jdk.internal.reflect.DirectConstructorHandleAccessor.newInstance(DirectConstructorHandleAccessor.java:62)
-	at java.base/java.lang.reflect.Constructor.newInstanceWithCaller(Constructor.java:502)
-	at java.base/java.lang.reflect.Constructor.newInstance(Constructor.java:486)
-	at org.openqa.selenium.remote.ErrorCodec.decode(ErrorCodec.java:167)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:138)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:50)
-	at org.openqa.selenium.remote.HttpCommandExecutor.execute(HttpCommandExecutor.java:215)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.invokeExecute(DriverCommandExecutor.java:216)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.execute(DriverCommandExecutor.java:174)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:544)
-	at org.openqa.selenium.remote.ElementLocation$ElementFinder$2.findElements(ElementLocation.java:182)
-	at org.openqa.selenium.remote.ElementLocation.findElements(ElementLocation.java:103)
-	at org.openqa.selenium.remote.RemoteWebDriver.findElements(RemoteWebDriver.java:380)
-	at org.openqa.selenium.remote.RemoteWebDriver.findElements(RemoteWebDriver.java:374)
-	at java.base/jdk.internal.reflect.DirectMethodHandleAccessor.invoke(DirectMethodHandleAccessor.java:103)
-	at java.base/java.lang.reflect.Method.invoke(Method.java:580)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.call(WebDriverDecorator.java:315)
-	at org.openqa.selenium.support.decorators.DefaultDecorated.call(DefaultDecorated.java:48)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.lambda$createProxyFactory$3(WebDriverDecorator.java:405)
-	at net.bytebuddy.renamed.java.lang.Object$ByteBuddy$8AV6NETA.findElements(Unknown Source)
-	at pages.AdminPanelSortingPage.lambda$3(AdminPanelSortingPage.java:723)
-	at org.openqa.selenium.support.ui.FluentWait.until(FluentWait.java:203)
-	at pages.AdminPanelSortingPage.verifyFirstProductInUserAppMicroPage(AdminPanelSortingPage.java:719)
-	at stepDef.AdminPanelSortingStepDef.i_should_see_the_same_product_appear_first_in_the_user_application_Micro_Page(AdminPanelSortingStepDef.java:65)
-	at ✽.I should see the same product appear first in the User Application Micro Page(file:///C:/Users/Sarojkumar/git/ZlaataQAsever/src/test/resources/features/AdminFeature/sortingProduct.feature:38)
-</t>
-  </si>
-  <si>
-    <t>stepDef.Hooks.tearDown(io.cucumber.java.Scenario)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.openqa.selenium.NoSuchWindowException: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=140.0.7339.129)
-Build info: version: '4.34.0', revision: '707dcb4246*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.8'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [6f42af8d51a245b62f759c30c0cc94cf, screenshot {}]
-Capabilities {acceptInsecureCerts: true, browserName: chrome, browserVersion: 140.0.7339.129, chrome: {chromedriverVersion: 140.0.7339.185 (eeea00e459e..., userDataDir: C:\Users\SAROJK~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52687}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52687/devtoo..., se:cdpVersion: 140.0.7339.129, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 6f42af8d51a245b62f759c30c0cc94cf
-	at java.base/jdk.internal.reflect.DirectConstructorHandleAccessor.newInstance(DirectConstructorHandleAccessor.java:62)
-	at java.base/java.lang.reflect.Constructor.newInstanceWithCaller(Constructor.java:502)
-	at java.base/java.lang.reflect.Constructor.newInstance(Constructor.java:486)
-	at org.openqa.selenium.remote.ErrorCodec.decode(ErrorCodec.java:167)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:138)
-	at org.openqa.selenium.remote.codec.w3c.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:50)
-	at org.openqa.selenium.remote.HttpCommandExecutor.execute(HttpCommandExecutor.java:215)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.invokeExecute(DriverCommandExecutor.java:216)
-	at org.openqa.selenium.remote.service.DriverCommandExecutor.execute(DriverCommandExecutor.java:174)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:544)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:617)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:621)
-	at org.openqa.selenium.remote.RemoteWebDriver.getScreenshotAs(RemoteWebDriver.java:333)
-	at java.base/jdk.internal.reflect.DirectMethodHandleAccessor.invoke(DirectMethodHandleAccessor.java:103)
-	at java.base/java.lang.reflect.Method.invoke(Method.java:580)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.call(WebDriverDecorator.java:315)
-	at org.openqa.selenium.support.decorators.DefaultDecorated.call(DefaultDecorated.java:48)
-	at org.openqa.selenium.support.decorators.WebDriverDecorator.lambda$createProxyFactory$3(WebDriverDecorator.java:405)
-	at net.bytebuddy.renamed.java.lang.Object$ByteBuddy$8AV6NETA.getScreenshotAs(Unknown Source)
-	at utils.ExcelReportUtil.captureScreenshot(ExcelReportUtil.java:68)
-	at stepDef.Hooks.tearDown(Hooks.java:298)
+    <t xml:space="preserve">java.lang.AssertionError: Products mismatch found.
+	at org.junit.Assert.fail(Assert.java:89)
+	at pages.AdminPanelExportExcelFileMatchPage.verifyExportedInactiveProductsMatch(AdminPanelExportExcelFileMatchPage.java:719)
+	at stepDef.AdminPanelExportExcelStepDef.i_verify_both_exported_inactive_products_files_and_have_matching_product_names(AdminPanelExportExcelStepDef.java:102)
+	at ✽.I verify both exported inactive products files "InactiveProducts1.xlsx" and "InactiveProducts2.xlsx" have matching product names(file:///C:/Users/Sarojkumar/git/ZlaataQAsever/src/test/resources/features/AdminFeature/exportExcelFile.feature:42)
 </t>
   </si>
 </sst>
@@ -939,7 +874,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1007,7 +942,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1075,7 +1010,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1302,7 +1237,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1369,7 +1304,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1436,7 +1371,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2601,7 +2536,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2668,7 +2603,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2735,7 +2670,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Admin Sorting The Product in Admin Panel Verify Successful Sort In User App.</c:v>
+                  <c:v>Admin Export The Excel File and Check with Veiw All Export Excel File Check Wheather its Matching .</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2964,7 +2899,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2975,7 +2910,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3036,7 +2971,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3103,7 +3038,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4082,7 +4017,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4093,7 +4028,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4154,7 +4089,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4221,7 +4156,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ASP_04 |Verify Micro Page product sorting between Admin Panel and User Application.| "TD_UI_Zlaata_ASP_04"</c:v>
+                  <c:v>TC_UI_Zlaata_EEF_04 |Verify Inactive Products match between two exports.| "TD_UI_Zlaata_EEF_04"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4637,7 +4572,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4704,7 +4639,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4771,7 +4706,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_ASP_04</c:v>
+                  <c:v>@TC_UI_Zlaata_EEF_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8546,7 +8481,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="DFD3" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="FE9B" scenarios="true" objects="true"/>
   <mergeCells count="8">
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="B61:C61"/>
@@ -8645,10 +8580,10 @@
         <v>40</v>
       </c>
       <c r="G22" s="50" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H22" s="55" t="n">
         <v>3.0</v>
-      </c>
-      <c r="H22" s="55" t="n">
-        <v>2.0</v>
       </c>
       <c r="I22" s="56" t="n">
         <v>1.0</v>
@@ -8885,10 +8820,10 @@
         <v>70</v>
       </c>
       <c r="J22" s="50" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K22" s="55" t="n">
         <v>3.0</v>
-      </c>
-      <c r="K22" s="55" t="n">
-        <v>2.0</v>
       </c>
       <c r="L22" s="56" t="n">
         <v>1.0</v>
@@ -8909,7 +8844,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="2.0" state="frozen" topLeftCell="A3" activePane="bottomLeft"/>
@@ -8952,22 +8887,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="true" password="CABF" scenarios="true" objects="true"/>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-  </mergeCells>
+  <sheetProtection sheet="true" password="8609" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9029,7 +8950,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -9101,7 +9022,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9203,7 +9124,7 @@
         <v>40</v>
       </c>
       <c r="R20" s="50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="S20" s="50" t="n">
         <v>1.0</v>

</xml_diff>